<commit_message>
Fix: Mulitple duplicate rendering of options while editing the questions
</commit_message>
<xml_diff>
--- a/public/report.xlsx
+++ b/public/report.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9" xml:space="preserve">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13" xml:space="preserve">
   <si>
     <t>Quiz name</t>
   </si>
@@ -36,6 +36,18 @@
   </si>
   <si>
     <t>alan@gaming.com</t>
+  </si>
+  <si>
+    <t>mayank@example.com</t>
+  </si>
+  <si>
+    <t>drax@galaxy.com</t>
+  </si>
+  <si>
+    <t>Solar system quiz</t>
+  </si>
+  <si>
+    <t>groot@galaxy.com</t>
   </si>
 </sst>
 </file>
@@ -99,13 +111,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView windowProtection="0" tabSelected="0" showWhiteSpace="0" showOutlineSymbols="0" showFormulas="0" rightToLeft="0" showZeros="1" showRuler="1" showRowColHeaders="1" showGridLines="1" defaultGridColor="1" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="1" customWidth="1" width="15.400000000000002"/>
+    <col min="1" max="1" bestFit="1" customWidth="1" width="22.0"/>
     <col min="2" max="2" bestFit="1" customWidth="1" width="13.200000000000001"/>
     <col min="3" max="3" bestFit="1" customWidth="1" width="25.3"/>
     <col min="4" max="4" bestFit="1" customWidth="1" width="19.8"/>
@@ -170,6 +182,51 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="0"/>
+      <c r="C5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0"/>
+      <c r="C6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="0"/>
+      <c r="C7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
   <printOptions verticalCentered="0" horizontalCentered="0" headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
Fix: Removed puts statement and fixed display of user name in downloaded excel file
</commit_message>
<xml_diff>
--- a/public/report.xlsx
+++ b/public/report.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9" xml:space="preserve">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24" xml:space="preserve">
   <si>
     <t>Quiz name</t>
   </si>
@@ -29,13 +29,58 @@
     <t>Solar system quiz</t>
   </si>
   <si>
+    <t>Mayank Agnihotri</t>
+  </si>
+  <si>
     <t>maxagno3@yahoo.com</t>
   </si>
   <si>
+    <t>Max Agno3</t>
+  </si>
+  <si>
     <t>manky@google.com</t>
   </si>
   <si>
+    <t>Max Trooper</t>
+  </si>
+  <si>
     <t>max@trooper.com</t>
+  </si>
+  <si>
+    <t>King Kong</t>
+  </si>
+  <si>
+    <t>kong@skullisland.com</t>
+  </si>
+  <si>
+    <t>Mech Godzilla</t>
+  </si>
+  <si>
+    <t>godzilla@kongvsgodzilla.com</t>
+  </si>
+  <si>
+    <t>Max Jax</t>
+  </si>
+  <si>
+    <t>max@jax.com</t>
+  </si>
+  <si>
+    <t>Max Steel</t>
+  </si>
+  <si>
+    <t>maxsteel@cartoonetwork.com</t>
+  </si>
+  <si>
+    <t>mayank@gmail.com</t>
+  </si>
+  <si>
+    <t>Tom Jerry</t>
+  </si>
+  <si>
+    <t>tomandjerry@cartoon.com</t>
+  </si>
+  <si>
+    <t>Gaming Quiz</t>
   </si>
 </sst>
 </file>
@@ -99,15 +144,15 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView windowProtection="0" tabSelected="0" showWhiteSpace="0" showOutlineSymbols="0" showFormulas="0" rightToLeft="0" showZeros="1" showRuler="1" showRowColHeaders="1" showGridLines="1" defaultGridColor="1" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" bestFit="1" customWidth="1" width="22.0"/>
-    <col min="2" max="2" bestFit="1" customWidth="1" width="13.200000000000001"/>
-    <col min="3" max="3" bestFit="1" customWidth="1" width="23.1"/>
+    <col min="2" max="2" bestFit="1" customWidth="1" width="20.900000000000002"/>
+    <col min="3" max="3" bestFit="1" customWidth="1" width="33.0"/>
     <col min="4" max="4" bestFit="1" customWidth="1" width="19.8"/>
     <col min="5" max="5" bestFit="1" customWidth="1" width="22.0"/>
   </cols>
@@ -133,9 +178,11 @@
       <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0"/>
+      <c r="B2" s="0" t="s">
+        <v>6</v>
+      </c>
       <c r="C2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>2</v>
@@ -148,9 +195,11 @@
       <c r="A3" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="0"/>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
       <c r="C3" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>0</v>
@@ -163,15 +212,136 @@
       <c r="A4" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="0"/>
+      <c r="B4" s="0" t="s">
+        <v>10</v>
+      </c>
       <c r="C4" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>